<commit_message>
add invoice and receipt
</commit_message>
<xml_diff>
--- a/cspa_invoice.xlsx
+++ b/cspa_invoice.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wing\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wing\temp\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -835,10 +835,10 @@
     <t>San Jose, CA 95170-0249</t>
   </si>
   <si>
-    <t>650 489-2772 / president@cspa.com / www.cspa.com</t>
-  </si>
-  <si>
     <t>TAX</t>
+  </si>
+  <si>
+    <t>650-489-2772 / president@cspa.com / www.cspa.com</t>
   </si>
 </sst>
 </file>
@@ -4673,7 +4673,7 @@
   <dimension ref="A1:BE55"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" showOutlineSymbols="0" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
@@ -4904,7 +4904,7 @@
       <c r="D5" s="76"/>
       <c r="E5" s="76"/>
       <c r="F5" s="158" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="G5" s="76"/>
       <c r="H5" s="76"/>
@@ -6779,7 +6779,7 @@
       <c r="G36" s="133"/>
       <c r="H36" s="133"/>
       <c r="I36" s="154" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J36" s="153">
         <v>0.09</v>
@@ -7846,7 +7846,7 @@
     <row r="5" spans="1:17">
       <c r="B5" s="34" t="str">
         <f>oknCompanyContact</f>
-        <v>650 489-2772 / president@cspa.com / www.cspa.com</v>
+        <v>650-489-2772 / president@cspa.com / www.cspa.com</v>
       </c>
       <c r="M5" s="23"/>
     </row>
@@ -8771,7 +8771,7 @@
       <c r="A5" s="16"/>
       <c r="B5" s="34" t="str">
         <f>oknCompanyContact</f>
-        <v>650 489-2772 / president@cspa.com / www.cspa.com</v>
+        <v>650-489-2772 / president@cspa.com / www.cspa.com</v>
       </c>
       <c r="M5" s="23"/>
       <c r="N5" s="37"/>
@@ -8963,7 +8963,7 @@
       <c r="A5" s="16"/>
       <c r="B5" s="34" t="str">
         <f>oknCompanyContact</f>
-        <v>650 489-2772 / president@cspa.com / www.cspa.com</v>
+        <v>650-489-2772 / president@cspa.com / www.cspa.com</v>
       </c>
       <c r="L5" s="35"/>
       <c r="M5" s="16"/>
@@ -9127,7 +9127,7 @@
       <c r="A5" s="16"/>
       <c r="B5" s="34" t="str">
         <f>oknCompanyContact</f>
-        <v>650 489-2772 / president@cspa.com / www.cspa.com</v>
+        <v>650-489-2772 / president@cspa.com / www.cspa.com</v>
       </c>
       <c r="D5" s="50"/>
       <c r="E5" s="50"/>
@@ -9360,7 +9360,7 @@
       <c r="A5" s="16"/>
       <c r="B5" s="34" t="str">
         <f>oknCompanyContact</f>
-        <v>650 489-2772 / president@cspa.com / www.cspa.com</v>
+        <v>650-489-2772 / president@cspa.com / www.cspa.com</v>
       </c>
       <c r="M5" s="23"/>
       <c r="N5" s="10"/>
@@ -9556,7 +9556,7 @@
       <c r="A5" s="16"/>
       <c r="B5" s="34" t="str">
         <f>oknCompanyContact</f>
-        <v>650 489-2772 / president@cspa.com / www.cspa.com</v>
+        <v>650-489-2772 / president@cspa.com / www.cspa.com</v>
       </c>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>

</xml_diff>